<commit_message>
This commit will perform lexical analysis, syntax analysis, semantic analysis, and the general structure of IR production
</commit_message>
<xml_diff>
--- a/Symbol_Table.xlsx
+++ b/Symbol_Table.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C98"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,12 +468,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t> </t>
+          <t>int</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>KEYWORD</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -483,12 +483,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>gcd</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>KEYWORD</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -498,12 +498,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t> </t>
+          <t>(</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>STR_BKT</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -513,12 +513,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>gcd</t>
+          <t>double</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>KEYWORD</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -528,12 +528,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>(</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>STR_BKT</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -543,12 +543,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>,</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>KEYWORD</t>
+          <t>COM</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -558,12 +558,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t> </t>
+          <t>int</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>KEYWORD</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -573,7 +573,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>b</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -588,12 +588,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>,</t>
+          <t>)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>COM</t>
+          <t>END_BKT</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -603,81 +603,88 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t> </t>
+          <t>if</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>KEYWORD</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>(</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>KEYWORD</t>
+          <t>STR_BKT</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t> </t>
+          <t>a</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="A15">
+        <f>=</f>
+        <v/>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>EV</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>)</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>END_BKT</t>
         </is>
       </c>
-      <c r="C16" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr"/>
       <c r="C17" t="n">
         <v>2</v>
       </c>
@@ -685,12 +692,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>	</t>
+          <t>then</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>KEYWORD</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -700,7 +707,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>if</t>
+          <t>return</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -743,13 +750,14 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22">
-        <f>=</f>
-        <v/>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>)</t>
+        </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>EV</t>
+          <t>END_BKT</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -759,12 +767,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>fi</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>KEYWORD</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -774,12 +782,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>)</t>
+          <t>;</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>END_BKT</t>
+          <t>SEMI</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -789,36 +797,44 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t> </t>
+          <t>if</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>KEYWORD</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>then</t>
+          <t>(</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>KEYWORD</t>
+          <t>STR_BKT</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr"/>
-      <c r="B27" t="inlineStr"/>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
       <c r="C27" t="n">
         <v>3</v>
       </c>
@@ -826,12 +842,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>	</t>
+          <t>&gt;</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>GT</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -839,8 +855,16 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr"/>
-      <c r="B29" t="inlineStr"/>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
       <c r="C29" t="n">
         <v>3</v>
       </c>
@@ -848,12 +872,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>	</t>
+          <t>)</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>END_BKT</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -863,7 +887,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>return</t>
+          <t>then</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -878,12 +902,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t> </t>
+          <t>return</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>KEYWORD</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -908,7 +932,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>gcd</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -923,12 +947,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>)</t>
+          <t>(</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>END_BKT</t>
+          <t>STR_BKT</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -938,12 +962,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t> </t>
+          <t>a</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -951,83 +975,99 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr"/>
-      <c r="B37" t="inlineStr"/>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>SUB</t>
+        </is>
+      </c>
       <c r="C37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>	</t>
+          <t>b</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>fi</t>
+          <t>,</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>KEYWORD</t>
+          <t>COM</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>;</t>
+          <t>b</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>END</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr"/>
-      <c r="B41" t="inlineStr"/>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>)</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>END_BKT</t>
+        </is>
+      </c>
       <c r="C41" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>	</t>
+          <t>)</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>END_BKT</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>if</t>
+          <t>else</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1036,162 +1076,178 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>(</t>
+          <t>return</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>STR_BKT</t>
+          <t>KEYWORD</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>(</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>STR_BKT</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>&gt;</t>
+          <t>gcd</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>GT</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>(</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>STR_BKT</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>)</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>END_BKT</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t> </t>
+          <t>,</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>COM</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>then</t>
+          <t>b</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>KEYWORD</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr"/>
-      <c r="B51" t="inlineStr"/>
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>SUB</t>
+        </is>
+      </c>
       <c r="C51" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>	</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr"/>
-      <c r="B53" t="inlineStr"/>
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>)</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>END_BKT</t>
+        </is>
+      </c>
       <c r="C53" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>	</t>
+          <t>)</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>END_BKT</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>return</t>
+          <t>fi</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1200,63 +1256,63 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>(</t>
+          <t>;</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>STR_BKT</t>
+          <t>SEMI</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>gcd</t>
+          <t>fed</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>KEYWORD</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>(</t>
+          <t>;</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>STR_BKT</t>
+          <t>SEMI</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>print</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>KEYWORD</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1266,12 +1322,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>gcd</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>SUB</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1281,12 +1337,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>(</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>STR_BKT</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1296,12 +1352,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>,</t>
+          <t>21</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>COM</t>
+          <t>INT</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1311,12 +1367,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>,</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>INT</t>
+          <t>COM</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1326,12 +1382,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>)</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>END_BKT</t>
+          <t>INT</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -1354,114 +1410,138 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr"/>
-      <c r="B66" t="inlineStr"/>
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>;</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>SEMI</t>
+        </is>
+      </c>
       <c r="C66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>	</t>
+          <t>print</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>KEYWORD</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>else</t>
+          <t>45</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>KEYWORD</t>
+          <t>INT</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t> </t>
+          <t>;</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>SEMI</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr"/>
-      <c r="B70" t="inlineStr"/>
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>print</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>KEYWORD</t>
+        </is>
+      </c>
       <c r="C70" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>	</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>INT</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr"/>
-      <c r="B72" t="inlineStr"/>
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>MLT</t>
+        </is>
+      </c>
       <c r="C72" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>	</t>
+          <t>(</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>STR_BKT</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>return</t>
+          <t>gcd</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>KEYWORD</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75">
@@ -1476,347 +1556,130 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>gcd</t>
+          <t>21</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>INT</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>(</t>
+          <t>,</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>STR_BKT</t>
+          <t>COM</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>28</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>INT</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>,</t>
+          <t>)</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>COM</t>
+          <t>END_BKT</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>+</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>ADD</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>SUB</t>
+          <t>INT</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>)</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>END_BKT</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>)</t>
+          <t>.</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>END_BKT</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>)</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>END_BKT</t>
-        </is>
-      </c>
-      <c r="C84" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>SPC</t>
-        </is>
-      </c>
-      <c r="C85" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr"/>
-      <c r="B86" t="inlineStr"/>
-      <c r="C86" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>	</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>SPC</t>
-        </is>
-      </c>
-      <c r="C87" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>fi</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>KEYWORD</t>
-        </is>
-      </c>
-      <c r="C88" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>;</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>END</t>
-        </is>
-      </c>
-      <c r="C89" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>fed</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>KEYWORD</t>
-        </is>
-      </c>
-      <c r="C90" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>;</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>END</t>
-        </is>
-      </c>
-      <c r="C91" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>print</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>KEYWORD</t>
-        </is>
-      </c>
-      <c r="C92" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>SPC</t>
-        </is>
-      </c>
-      <c r="C93" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>gcd</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="C94" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>(</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>STR_BKT</t>
-        </is>
-      </c>
-      <c r="C95" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>INT</t>
-        </is>
-      </c>
-      <c r="C96" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>,</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>COM</t>
-        </is>
-      </c>
-      <c r="C97" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>INT</t>
-        </is>
-      </c>
-      <c r="C98" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>